<commit_message>
🤖 Auto scrape: 2025-08-15 05:27:12
</commit_message>
<xml_diff>
--- a/data/08_15_25_tradewheel_scrap.xlsx
+++ b/data/08_15_25_tradewheel_scrap.xlsx
@@ -482,7 +482,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24 minutes ago</t>
+          <t>31 minutes ago</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -502,7 +502,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -534,7 +534,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -662,7 +662,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -694,7 +694,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -790,7 +790,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -822,7 +822,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -918,7 +918,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -982,7 +982,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16 hours ago</t>
+          <t>17 hours ago</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16 hours ago</t>
+          <t>17 hours ago</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16 hours ago</t>
+          <t>17 hours ago</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1782,7 +1782,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1878,7 +1878,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1942,7 +1942,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>17 hours ago</t>
+          <t>18 hours ago</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2358,7 +2358,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2454,7 +2454,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2486,7 +2486,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2550,7 +2550,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2582,7 +2582,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2614,7 +2614,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2742,7 +2742,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2774,7 +2774,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2806,7 +2806,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2870,7 +2870,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2902,7 +2902,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2966,7 +2966,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3094,7 +3094,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3158,7 +3158,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3190,7 +3190,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3286,7 +3286,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3318,7 +3318,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3350,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3414,7 +3414,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3574,7 +3574,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3638,7 +3638,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3702,7 +3702,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3862,7 +3862,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4022,7 +4022,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4118,7 +4118,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4278,7 +4278,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4310,7 +4310,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4342,7 +4342,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4470,7 +4470,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4502,7 +4502,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4598,7 +4598,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4662,7 +4662,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4790,7 +4790,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4950,7 +4950,7 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5046,7 +5046,7 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5078,7 +5078,7 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5110,7 +5110,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5142,7 +5142,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5206,7 +5206,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5238,7 +5238,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5270,7 +5270,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5302,7 +5302,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5430,7 +5430,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5494,7 +5494,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5558,7 +5558,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5590,7 +5590,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5622,7 +5622,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5654,7 +5654,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5718,7 +5718,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5750,7 +5750,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5782,7 +5782,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5814,7 +5814,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5910,7 +5910,7 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5942,7 +5942,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6006,7 +6006,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6070,7 +6070,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6166,7 +6166,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6198,7 +6198,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6230,7 +6230,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6262,7 +6262,7 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6326,7 +6326,7 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6358,7 +6358,7 @@
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6390,7 +6390,7 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6422,7 +6422,7 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6454,7 +6454,7 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6486,7 +6486,7 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6518,7 +6518,7 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6550,7 +6550,7 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6582,7 +6582,7 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6614,7 +6614,7 @@
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6646,7 +6646,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6678,7 +6678,7 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6710,7 +6710,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6742,7 +6742,7 @@
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6774,7 +6774,7 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6806,7 +6806,7 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>2025-08-15 12:18:02</t>
+          <t>2025-08-15 12:25:01</t>
         </is>
       </c>
     </row>

</xml_diff>